<commit_message>
jeux de test avec avancement sur java
</commit_message>
<xml_diff>
--- a/jeu de test.xlsx
+++ b/jeu de test.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
   <si>
     <t>Action</t>
   </si>
@@ -191,16 +190,102 @@
   </si>
   <si>
     <t>Exception: produit n'existe plus</t>
+  </si>
+  <si>
+    <t>modifier un article</t>
+  </si>
+  <si>
+    <t>modifier le nombre d'article en stock</t>
+  </si>
+  <si>
+    <t>augmentation nb d'article en stock</t>
+  </si>
+  <si>
+    <t>diminution nb d'aticle en stock (nb darticle&lt;0)</t>
+  </si>
+  <si>
+    <t>diminution nb d'aticle en stock (nb darticle&gt;0)</t>
+  </si>
+  <si>
+    <t>diminution nb d'aticle en stock (nb darticle=0)</t>
+  </si>
+  <si>
+    <t>OK ajout de la mention rupture de stock</t>
+  </si>
+  <si>
+    <t>Ajouter un article</t>
+  </si>
+  <si>
+    <t>Tous les champs sont renseigner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer un avis </t>
+  </si>
+  <si>
+    <t>Exception: Avis en cours de consultation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Exception: Nombre article négatif </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>OU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>OK Nb article = 0</t>
+    </r>
+  </si>
+  <si>
+    <t>Avis en cours de cosultation par une tiers personne</t>
+  </si>
+  <si>
+    <t>OK mais garde une trace de l'article dans la BD</t>
+  </si>
+  <si>
+    <t>Connection</t>
+  </si>
+  <si>
+    <t>mots de passe non concordent avec le UserName</t>
+  </si>
+  <si>
+    <t>Exception: Administrateur non reconnu</t>
+  </si>
+  <si>
+    <t>Création de compte</t>
+  </si>
+  <si>
+    <t>tous les champs sont rempli + un administrateur déjà existant tape sont mot de passe personnel</t>
+  </si>
+  <si>
+    <t>JE SAIS PAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -209,22 +294,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -245,8 +315,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,9 +352,15 @@
         <bgColor rgb="FF800080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -281,69 +368,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -402,310 +449,605 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="54.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.9897959183674"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7295918367347"/>
+    <col min="1" max="2" width="54.42578125"/>
+    <col min="3" max="3" width="67"/>
+    <col min="4" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>52</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>55</v>
       </c>
@@ -716,82 +1058,147 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A29:C29"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7295918367347"/>
+    <col min="1" max="1025" width="10.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7295918367347"/>
+    <col min="1" max="1025" width="10.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>